<commit_message>
Added the package latest version 0.1.2
</commit_message>
<xml_diff>
--- a/Files/EXCEL Output/ASSIGNMENT_EMP0222_DATAFLOW.xlsx
+++ b/Files/EXCEL Output/ASSIGNMENT_EMP0222_DATAFLOW.xlsx
@@ -130,8 +130,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Source" displayName="Source" ref="A1:I2" headerRowCount="1">
-  <autoFilter ref="A1:I2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Source" displayName="Source" ref="A1:I3" headerRowCount="1">
+  <autoFilter ref="A1:I3"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Table No"/>
     <tableColumn id="2" name="Table Name"/>
@@ -533,7 +533,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
@@ -552,7 +552,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Workspaces = Source{[Id="Workspaces"]}[Data],</t>
+          <t xml:space="preserve"> PowerPlatform.Dataflows(null),</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -575,9 +575,9 @@
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">1. This ID is associated with a specific workspace containing data.
-2. #"616fac86-19ac-40a2-85bb-15d517e1076f" is associated with dataflow "a025ea09-ff3a-40c4-9033-a14f69c30f0a" and contains data.
-3. Financials (2) is a type of data with the identifier "a025ea09-ff3a-40c4-9033-a14f69c30f0a".
+          <t xml:space="preserve">1. This is an identification for a workspace, which contains data within it.
+2. The dataflow ID "a025ea09-ff3a-40c4-9033-a14f69c30f0a" is equal to "616fac86-19ac-40a2-85bb-15d517e1076f" with the Data attribute set
+3. "financials (2)" refers to a particular version of financial data.
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
Added the PyPbitExtractor Package
</commit_message>
<xml_diff>
--- a/Files/EXCEL Output/ASSIGNMENT_EMP0222_DATAFLOW.xlsx
+++ b/Files/EXCEL Output/ASSIGNMENT_EMP0222_DATAFLOW.xlsx
@@ -575,9 +575,9 @@
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">1. This is an identification for a workspace, which contains data within it.
-2. The dataflow ID "a025ea09-ff3a-40c4-9033-a14f69c30f0a" is equal to "616fac86-19ac-40a2-85bb-15d517e1076f" with the Data attribute set
-3. "financials (2)" refers to a particular version of financial data.
+          <t xml:space="preserve">1. This is the ID of a workspace containing data.
+2. The dataflowId "a025ea09-ff3a-40c4-9033-a14f69c30f0a" is associated with data identified by the identifier "616fac86-19ac-40a2-85bb-15d517e1076f".
+3. Financials (2) refers to a specific set of numerical data relating to a company's financial standing.
 </t>
         </is>
       </c>

</xml_diff>